<commit_message>
Added Spirals graph, filled the collected data for the optimized runs
</commit_message>
<xml_diff>
--- a/collected_data.xlsx
+++ b/collected_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Undergraduate/16th Grade/Spring/Machine Learning/Projects/Project 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{9557476C-02A0-4340-9C51-B94372527253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E0B2D43-4A17-4135-9DB3-3844F9DC8F76}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{9557476C-02A0-4340-9C51-B94372527253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A39FE70-E504-48B4-B83E-572DA19BC9A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C16E27F3-1A5E-4519-9C57-8640C94CB8B1}"/>
   </bookViews>
@@ -35,15 +35,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+  <si>
+    <t>Blobs</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Digits</t>
+  </si>
+  <si>
+    <t>Letters</t>
+  </si>
+  <si>
+    <t>Number of Examples (In-Depth Runs)</t>
+  </si>
+  <si>
+    <t>Number of Examples (Optimized Single Run)</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Spirals</t>
+  </si>
+  <si>
+    <t>Zoo</t>
+  </si>
+  <si>
+    <t>Average Training Set Accuracy (%)</t>
+  </si>
+  <si>
+    <t>Average Testing Set Accuracy (%)</t>
+  </si>
   <si>
     <t>Average Time Elapsed (s)</t>
   </si>
   <si>
-    <t>Average Training Set Accuracy (%)</t>
-  </si>
-  <si>
-    <t>Average Testing Set Accuracy (%)</t>
+    <t>Max Depth</t>
+  </si>
+  <si>
+    <t>Min Examples</t>
+  </si>
+  <si>
+    <t>Min Proportion</t>
+  </si>
+  <si>
+    <t>Num Trees</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -79,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,31 +438,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F756A3E-CD9F-483F-95CB-92A161BC6F35}">
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1">
+        <v>500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2500</v>
+      </c>
+      <c r="D2" s="1">
+        <v>83.51</v>
+      </c>
+      <c r="E2" s="1">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="F2" s="1">
+        <v>100.68</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>600</v>
+      </c>
+      <c r="C3" s="1">
+        <v>600</v>
+      </c>
+      <c r="D3" s="1">
+        <v>95.88</v>
+      </c>
+      <c r="E3" s="1">
+        <v>94</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.61</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>80</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" s="1">
+        <v>250</v>
+      </c>
+      <c r="C4" s="1">
+        <v>250</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="F4" s="1">
+        <v>35.630000000000003</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>500</v>
+      </c>
+      <c r="D5" s="1">
+        <v>99.9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>67.8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>47.29</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
         <v>0</v>
       </c>
+      <c r="C6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>96.7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>46.39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>97</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added impurity data to collected data
</commit_message>
<xml_diff>
--- a/collected_data.xlsx
+++ b/collected_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Undergraduate/16th Grade/Spring/Machine Learning/Projects/Project 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{9557476C-02A0-4340-9C51-B94372527253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A39FE70-E504-48B4-B83E-572DA19BC9A6}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{9557476C-02A0-4340-9C51-B94372527253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E35C915-5016-497F-87B8-3710B4AFE484}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C16E27F3-1A5E-4519-9C57-8640C94CB8B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C16E27F3-1A5E-4519-9C57-8640C94CB8B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameter Tuning" sheetId="1" r:id="rId1"/>
+    <sheet name="Optimal Single Run" sheetId="2" r:id="rId2"/>
+    <sheet name="Impurity Measures" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
   <si>
     <t>Blobs</t>
   </si>
@@ -49,12 +51,6 @@
     <t>Letters</t>
   </si>
   <si>
-    <t>Number of Examples (In-Depth Runs)</t>
-  </si>
-  <si>
-    <t>Number of Examples (Optimized Single Run)</t>
-  </si>
-  <si>
     <t>Dataset</t>
   </si>
   <si>
@@ -86,6 +82,24 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Number of Examples</t>
+  </si>
+  <si>
+    <t>Impurity Measure</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Impurtity Measure</t>
+  </si>
+  <si>
+    <t>Misclassification</t>
+  </si>
+  <si>
+    <t>Gini</t>
   </si>
 </sst>
 </file>
@@ -438,258 +452,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F756A3E-CD9F-483F-95CB-92A161BC6F35}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>500</v>
       </c>
-      <c r="C2" s="1">
-        <v>2500</v>
-      </c>
-      <c r="D2" s="1">
-        <v>83.51</v>
-      </c>
-      <c r="E2" s="1">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="F2" s="1">
-        <v>100.68</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>600</v>
       </c>
-      <c r="C3" s="1">
-        <v>600</v>
-      </c>
-      <c r="D3" s="1">
-        <v>95.88</v>
-      </c>
-      <c r="E3" s="1">
-        <v>94</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3.61</v>
-      </c>
-      <c r="G3" s="1">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1">
-        <v>80</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="J3" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>250</v>
       </c>
-      <c r="C4" s="1">
-        <v>250</v>
-      </c>
-      <c r="D4" s="1">
-        <v>100</v>
-      </c>
-      <c r="E4" s="1">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="F4" s="1">
-        <v>35.630000000000003</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>500</v>
       </c>
-      <c r="C5" s="1">
-        <v>500</v>
-      </c>
-      <c r="D5" s="1">
-        <v>99.9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>67.8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>47.29</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1">
-        <v>96.7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>46.39</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>101</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1">
-        <v>97</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J8" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
     <sortCondition ref="A2:A7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFE1421-D486-4F70-BE89-A8DD07CE35BC}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C2" s="1">
+        <v>83.51</v>
+      </c>
+      <c r="D2" s="1">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100.68</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>600</v>
+      </c>
+      <c r="C3" s="1">
+        <v>95.88</v>
+      </c>
+      <c r="D3" s="1">
+        <v>94</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.61</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>80</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>250</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="E4" s="1">
+        <v>35.630000000000003</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1">
+        <v>150</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>99.9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>67.8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>47.29</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1">
+        <v>100</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>96.7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46.39</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>97</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1">
+        <v>150</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8D2822-B742-4F33-9DC6-5408FD4F68D6}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+      <c r="C2" s="1">
+        <v>95.33</v>
+      </c>
+      <c r="D2" s="1">
+        <v>94.17</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>80</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I2" s="1">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>600</v>
+      </c>
+      <c r="C3" s="1">
+        <v>95.42</v>
+      </c>
+      <c r="D3" s="1">
+        <v>93.83</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>80</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>600</v>
+      </c>
+      <c r="C4" s="1">
+        <v>95.46</v>
+      </c>
+      <c r="D4" s="1">
+        <v>94.17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.94</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>80</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>250</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>61.2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>30.18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1">
+        <v>150</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>250</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>70.8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>33.590000000000003</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1">
+        <v>150</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>250</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>73.2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>34.92</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1">
+        <v>150</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>